<commit_message>
fixed the web page rendering to support blank nodes in the graph
</commit_message>
<xml_diff>
--- a/tests/catalog.xlsx
+++ b/tests/catalog.xlsx
@@ -732,7 +732,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
+      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -996,6 +996,12 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J1:J1006" type="date">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="jdoe@example.com"/>
     <hyperlink ref="F2" r:id="rId2" display="https://creativecommons.org/licenses/by/4.0/"/>

</xml_diff>